<commit_message>
Correccion de error, agrega d si d' esta presente en toda la cadena, agrega descripcion del algoritmo 3
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joose\Desktop\F2L\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFED3756-E701-4C59-9F98-2B31509743B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0282B030-43F7-4378-AEC4-A84E107528EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2799" uniqueCount="1065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2800" uniqueCount="1066">
   <si>
     <t>U R U' R'</t>
   </si>
@@ -3231,6 +3231,9 @@
   </si>
   <si>
     <t>r U r' U r U2 r' U' r U' r'</t>
+  </si>
+  <si>
+    <t>Alternative Algorithm 2 or Case from another angle.</t>
   </si>
 </sst>
 </file>
@@ -3572,7 +3575,7 @@
   <dimension ref="A1:J408"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3639,6 +3642,9 @@
       <c r="G2" t="s">
         <v>68</v>
       </c>
+      <c r="H2" t="s">
+        <v>1065</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Actualización de generador de documento, creacion de una base de datos para hacer pruebas, ampliacion de base de datos
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joose\Desktop\F2L\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0282B030-43F7-4378-AEC4-A84E107528EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829A7D17-B2E1-47E7-B175-6E4735DD2A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2800" uniqueCount="1066">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2840" uniqueCount="1078">
   <si>
     <t>U R U' R'</t>
   </si>
@@ -3234,6 +3234,42 @@
   </si>
   <si>
     <t>Alternative Algorithm 2 or Case from another angle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Useful Cases Name or </t>
+  </si>
+  <si>
+    <t>Alternative algorithm or warnings</t>
+  </si>
+  <si>
+    <t>UF2L22</t>
+  </si>
+  <si>
+    <t>R U R' L' U' L</t>
+  </si>
+  <si>
+    <t>UF2L23</t>
+  </si>
+  <si>
+    <t>L' U' L R U R'</t>
+  </si>
+  <si>
+    <t>UF2L24</t>
+  </si>
+  <si>
+    <t>R U R' r' U' R U M'</t>
+  </si>
+  <si>
+    <t>UF2L25</t>
+  </si>
+  <si>
+    <t>R U R' f R f'</t>
+  </si>
+  <si>
+    <t>UF2L26</t>
+  </si>
+  <si>
+    <t>D' L' U L D</t>
   </si>
 </sst>
 </file>
@@ -3572,10 +3608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J408"/>
+  <dimension ref="A1:J414"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A386" workbookViewId="0">
+      <selection activeCell="F389" sqref="F389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13093,7 +13129,7 @@
         <v>504</v>
       </c>
       <c r="D354" t="str">
-        <f t="shared" ref="D354:D408" si="7">E354 &amp; "_" &amp; B354 &amp; ".png"</f>
+        <f t="shared" ref="D354:D387" si="7">E354 &amp; "_" &amp; B354 &amp; ".png"</f>
         <v>AF2L21_Back Right.png</v>
       </c>
       <c r="E354" t="s">
@@ -14064,23 +14100,26 @@
         <v>1007</v>
       </c>
       <c r="B388" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="C388" t="s">
-        <v>1008</v>
+        <v>65</v>
       </c>
       <c r="D388" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L1_Front Right.png</v>
+        <f t="shared" ref="D388:D412" si="8">E388 &amp; "_" &amp; B388 &amp; ".png"</f>
+        <v>Useful Cases Name or _Working Slot.png</v>
       </c>
       <c r="E388" t="s">
-        <v>1009</v>
+        <v>1066</v>
       </c>
       <c r="F388" t="s">
-        <v>1020</v>
-      </c>
-      <c r="I388" s="2" t="s">
-        <v>459</v>
+        <v>67</v>
+      </c>
+      <c r="G388" t="s">
+        <v>1067</v>
+      </c>
+      <c r="I388" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="389" spans="1:9" x14ac:dyDescent="0.35">
@@ -14094,17 +14133,17 @@
         <v>1008</v>
       </c>
       <c r="D389" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L2_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L1_Front Right.png</v>
       </c>
       <c r="E389" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F389" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="I389" s="2" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
     </row>
     <row r="390" spans="1:9" x14ac:dyDescent="0.35">
@@ -14118,17 +14157,17 @@
         <v>1008</v>
       </c>
       <c r="D390" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L3_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L2_Front Right.png</v>
       </c>
       <c r="E390" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F390" t="s">
-        <v>955</v>
+        <v>1021</v>
       </c>
       <c r="I390" s="2" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="391" spans="1:9" x14ac:dyDescent="0.35">
@@ -14142,17 +14181,17 @@
         <v>1008</v>
       </c>
       <c r="D391" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L4_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L3_Front Right.png</v>
       </c>
       <c r="E391" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="F391" t="s">
-        <v>696</v>
+        <v>955</v>
       </c>
       <c r="I391" s="2" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
     </row>
     <row r="392" spans="1:9" x14ac:dyDescent="0.35">
@@ -14163,20 +14202,20 @@
         <v>22</v>
       </c>
       <c r="C392" t="s">
-        <v>1022</v>
+        <v>1008</v>
       </c>
       <c r="D392" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L5_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L4_Front Right.png</v>
       </c>
       <c r="E392" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="F392" t="s">
-        <v>1023</v>
+        <v>696</v>
       </c>
       <c r="I392" s="2" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="393" spans="1:9" x14ac:dyDescent="0.35">
@@ -14190,17 +14229,17 @@
         <v>1022</v>
       </c>
       <c r="D393" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L6_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L5_Front Right.png</v>
       </c>
       <c r="E393" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="F393" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I393" s="2" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
     </row>
     <row r="394" spans="1:9" x14ac:dyDescent="0.35">
@@ -14214,14 +14253,14 @@
         <v>1022</v>
       </c>
       <c r="D394" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L7_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L6_Front Right.png</v>
       </c>
       <c r="E394" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="F394" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I394" s="2" t="s">
         <v>451</v>
@@ -14238,17 +14277,17 @@
         <v>1022</v>
       </c>
       <c r="D395" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L8_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L7_Front Right.png</v>
       </c>
       <c r="E395" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="F395" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="I395" s="2" t="s">
-        <v>612</v>
+        <v>451</v>
       </c>
     </row>
     <row r="396" spans="1:9" x14ac:dyDescent="0.35">
@@ -14262,14 +14301,14 @@
         <v>1022</v>
       </c>
       <c r="D396" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L9_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L8_Front Right.png</v>
       </c>
       <c r="E396" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="F396" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="I396" s="2" t="s">
         <v>612</v>
@@ -14283,17 +14322,17 @@
         <v>22</v>
       </c>
       <c r="C397" t="s">
-        <v>1028</v>
+        <v>1022</v>
       </c>
       <c r="D397" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L10_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L9_Front Right.png</v>
       </c>
       <c r="E397" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="F397" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="I397" s="2" t="s">
         <v>612</v>
@@ -14310,14 +14349,14 @@
         <v>1028</v>
       </c>
       <c r="D398" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L11_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L10_Front Right.png</v>
       </c>
       <c r="E398" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="F398" t="s">
-        <v>112</v>
+        <v>1029</v>
       </c>
       <c r="I398" s="2" t="s">
         <v>612</v>
@@ -14331,17 +14370,17 @@
         <v>22</v>
       </c>
       <c r="C399" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="D399" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L12_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L11_Front Right.png</v>
       </c>
       <c r="E399" t="s">
-        <v>1031</v>
+        <v>1019</v>
       </c>
       <c r="F399" t="s">
-        <v>1034</v>
+        <v>112</v>
       </c>
       <c r="I399" s="2" t="s">
         <v>612</v>
@@ -14358,17 +14397,17 @@
         <v>1030</v>
       </c>
       <c r="D400" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L13_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L12_Front Right.png</v>
       </c>
       <c r="E400" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="F400" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="I400" s="2" t="s">
-        <v>451</v>
+        <v>612</v>
       </c>
     </row>
     <row r="401" spans="1:9" x14ac:dyDescent="0.35">
@@ -14379,20 +14418,20 @@
         <v>22</v>
       </c>
       <c r="C401" t="s">
-        <v>1036</v>
+        <v>1030</v>
       </c>
       <c r="D401" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L14_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L13_Front Right.png</v>
       </c>
       <c r="E401" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="F401" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="I401" s="2" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="402" spans="1:9" x14ac:dyDescent="0.35">
@@ -14406,20 +14445,17 @@
         <v>1036</v>
       </c>
       <c r="D402" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L15_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L14_Front Right.png</v>
       </c>
       <c r="E402" t="s">
-        <v>1039</v>
+        <v>1033</v>
       </c>
       <c r="F402" t="s">
-        <v>1040</v>
-      </c>
-      <c r="G402" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
       <c r="I402" s="2" t="s">
-        <v>612</v>
+        <v>459</v>
       </c>
     </row>
     <row r="403" spans="1:9" x14ac:dyDescent="0.35">
@@ -14433,20 +14469,20 @@
         <v>1036</v>
       </c>
       <c r="D403" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L16_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L15_Front Right.png</v>
       </c>
       <c r="E403" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="F403" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="G403" t="s">
-        <v>1050</v>
+        <v>1041</v>
       </c>
       <c r="I403" s="2" t="s">
-        <v>451</v>
+        <v>612</v>
       </c>
     </row>
     <row r="404" spans="1:9" x14ac:dyDescent="0.35">
@@ -14460,17 +14496,20 @@
         <v>1036</v>
       </c>
       <c r="D404" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L17_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L16_Front Right.png</v>
       </c>
       <c r="E404" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="F404" t="s">
-        <v>1044</v>
+        <v>1042</v>
+      </c>
+      <c r="G404" t="s">
+        <v>1050</v>
       </c>
       <c r="I404" s="2" t="s">
-        <v>612</v>
+        <v>451</v>
       </c>
     </row>
     <row r="405" spans="1:9" x14ac:dyDescent="0.35">
@@ -14484,14 +14523,14 @@
         <v>1036</v>
       </c>
       <c r="D405" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L18_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L17_Front Right.png</v>
       </c>
       <c r="E405" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="F405" t="s">
-        <v>1038</v>
+        <v>1044</v>
       </c>
       <c r="I405" s="2" t="s">
         <v>612</v>
@@ -14508,17 +14547,14 @@
         <v>1036</v>
       </c>
       <c r="D406" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L19_Front Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L18_Front Right.png</v>
       </c>
       <c r="E406" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="F406" t="s">
-        <v>1060</v>
-      </c>
-      <c r="G406" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
       <c r="I406" s="2" t="s">
         <v>612</v>
@@ -14529,26 +14565,26 @@
         <v>1007</v>
       </c>
       <c r="B407" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C407" t="s">
         <v>1036</v>
       </c>
       <c r="D407" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L20_Back Right.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L19_Front Right.png</v>
       </c>
       <c r="E407" t="s">
-        <v>1059</v>
+        <v>1048</v>
       </c>
       <c r="F407" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="G407" t="s">
-        <v>1050</v>
+        <v>1041</v>
       </c>
       <c r="I407" s="2" t="s">
-        <v>451</v>
+        <v>612</v>
       </c>
     </row>
     <row r="408" spans="1:9" x14ac:dyDescent="0.35">
@@ -14556,25 +14592,181 @@
         <v>1007</v>
       </c>
       <c r="B408" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="C408" t="s">
-        <v>1047</v>
+        <v>1036</v>
       </c>
       <c r="D408" t="str">
-        <f t="shared" si="7"/>
-        <v>UF2L21_Front Left.png</v>
+        <f t="shared" si="8"/>
+        <v>UF2L20_Back Right.png</v>
       </c>
       <c r="E408" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="F408" t="s">
-        <v>1049</v>
+        <v>1062</v>
       </c>
       <c r="G408" t="s">
         <v>1050</v>
       </c>
       <c r="I408" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="409" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A409" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B409" t="s">
+        <v>22</v>
+      </c>
+      <c r="C409" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D409" t="str">
+        <f t="shared" si="8"/>
+        <v>UF2L21_Front Right.png</v>
+      </c>
+      <c r="E409" t="s">
+        <v>1061</v>
+      </c>
+      <c r="F409" t="s">
+        <v>1069</v>
+      </c>
+      <c r="I409" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="410" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A410" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B410" t="s">
+        <v>24</v>
+      </c>
+      <c r="C410" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D410" t="str">
+        <f t="shared" si="8"/>
+        <v>UF2L22_Front Left.png</v>
+      </c>
+      <c r="E410" t="s">
+        <v>1068</v>
+      </c>
+      <c r="F410" t="s">
+        <v>1071</v>
+      </c>
+      <c r="I410" s="2" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="411" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A411" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B411" t="s">
+        <v>22</v>
+      </c>
+      <c r="C411" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D411" t="str">
+        <f t="shared" si="8"/>
+        <v>UF2L23_Front Right.png</v>
+      </c>
+      <c r="E411" t="s">
+        <v>1070</v>
+      </c>
+      <c r="F411" t="s">
+        <v>1073</v>
+      </c>
+      <c r="G411" t="s">
+        <v>1050</v>
+      </c>
+      <c r="I411" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="412" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A412" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B412" t="s">
+        <v>22</v>
+      </c>
+      <c r="C412" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D412" t="str">
+        <f t="shared" si="8"/>
+        <v>UF2L24_Front Right.png</v>
+      </c>
+      <c r="E412" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F412" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G412" t="s">
+        <v>1050</v>
+      </c>
+      <c r="I412" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="413" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A413" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B413" t="s">
+        <v>24</v>
+      </c>
+      <c r="C413" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D413" t="str">
+        <f>E413 &amp; "_" &amp; B413 &amp; ".png"</f>
+        <v>UF2L25_Front Left.png</v>
+      </c>
+      <c r="E413" t="s">
+        <v>1074</v>
+      </c>
+      <c r="F413" t="s">
+        <v>1049</v>
+      </c>
+      <c r="G413" t="s">
+        <v>1050</v>
+      </c>
+      <c r="I413" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="414" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A414" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B414" t="s">
+        <v>24</v>
+      </c>
+      <c r="C414" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D414" t="str">
+        <f>E414 &amp; "_" &amp; B414 &amp; ".png"</f>
+        <v>UF2L26_Front Left.png</v>
+      </c>
+      <c r="E414" t="s">
+        <v>1076</v>
+      </c>
+      <c r="F414" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G414" t="s">
+        <v>1050</v>
+      </c>
+      <c r="I414" s="2" t="s">
         <v>459</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Por ahora, el codigo esta terminado y ya ha acabado
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joose\Desktop\F2L\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829A7D17-B2E1-47E7-B175-6E4735DD2A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9A951C-773C-49D3-B49F-88EBDFC32E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2840" uniqueCount="1078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2847" uniqueCount="1081">
   <si>
     <t>U R U' R'</t>
   </si>
@@ -3270,6 +3270,15 @@
   </si>
   <si>
     <t>D' L' U L D</t>
+  </si>
+  <si>
+    <t>UF2L27</t>
+  </si>
+  <si>
+    <t>R' D' F D R</t>
+  </si>
+  <si>
+    <t>R' u' R u R</t>
   </si>
 </sst>
 </file>
@@ -3608,10 +3617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J414"/>
+  <dimension ref="A1:J415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A386" workbookViewId="0">
-      <selection activeCell="F389" sqref="F389"/>
+    <sheetView tabSelected="1" topLeftCell="A396" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F405" sqref="F405"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14106,7 +14115,7 @@
         <v>65</v>
       </c>
       <c r="D388" t="str">
-        <f t="shared" ref="D388:D412" si="8">E388 &amp; "_" &amp; B388 &amp; ".png"</f>
+        <f t="shared" ref="D388:D405" si="8">E388 &amp; "_" &amp; B388 &amp; ".png"</f>
         <v>Useful Cases Name or _Working Slot.png</v>
       </c>
       <c r="E388" t="s">
@@ -14530,10 +14539,13 @@
         <v>1045</v>
       </c>
       <c r="F405" t="s">
-        <v>1044</v>
+        <v>1079</v>
+      </c>
+      <c r="G405" t="s">
+        <v>1080</v>
       </c>
       <c r="I405" s="2" t="s">
-        <v>612</v>
+        <v>459</v>
       </c>
     </row>
     <row r="406" spans="1:9" x14ac:dyDescent="0.35">
@@ -14547,14 +14559,14 @@
         <v>1036</v>
       </c>
       <c r="D406" t="str">
-        <f t="shared" si="8"/>
+        <f>E406 &amp; "_" &amp; B406 &amp; ".png"</f>
         <v>UF2L18_Front Right.png</v>
       </c>
       <c r="E406" t="s">
         <v>1046</v>
       </c>
       <c r="F406" t="s">
-        <v>1038</v>
+        <v>1044</v>
       </c>
       <c r="I406" s="2" t="s">
         <v>612</v>
@@ -14571,17 +14583,14 @@
         <v>1036</v>
       </c>
       <c r="D407" t="str">
-        <f t="shared" si="8"/>
+        <f>E407 &amp; "_" &amp; B407 &amp; ".png"</f>
         <v>UF2L19_Front Right.png</v>
       </c>
       <c r="E407" t="s">
         <v>1048</v>
       </c>
       <c r="F407" t="s">
-        <v>1060</v>
-      </c>
-      <c r="G407" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
       <c r="I407" s="2" t="s">
         <v>612</v>
@@ -14592,26 +14601,26 @@
         <v>1007</v>
       </c>
       <c r="B408" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="C408" t="s">
         <v>1036</v>
       </c>
       <c r="D408" t="str">
-        <f t="shared" si="8"/>
-        <v>UF2L20_Back Right.png</v>
+        <f>E408 &amp; "_" &amp; B408 &amp; ".png"</f>
+        <v>UF2L20_Front Right.png</v>
       </c>
       <c r="E408" t="s">
         <v>1059</v>
       </c>
       <c r="F408" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="G408" t="s">
-        <v>1050</v>
+        <v>1041</v>
       </c>
       <c r="I408" s="2" t="s">
-        <v>451</v>
+        <v>612</v>
       </c>
     </row>
     <row r="409" spans="1:9" x14ac:dyDescent="0.35">
@@ -14619,23 +14628,26 @@
         <v>1007</v>
       </c>
       <c r="B409" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C409" t="s">
         <v>1036</v>
       </c>
       <c r="D409" t="str">
-        <f t="shared" si="8"/>
-        <v>UF2L21_Front Right.png</v>
+        <f>E409 &amp; "_" &amp; B409 &amp; ".png"</f>
+        <v>UF2L21_Back Right.png</v>
       </c>
       <c r="E409" t="s">
         <v>1061</v>
       </c>
       <c r="F409" t="s">
-        <v>1069</v>
+        <v>1062</v>
+      </c>
+      <c r="G409" t="s">
+        <v>1050</v>
       </c>
       <c r="I409" s="2" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="410" spans="1:9" x14ac:dyDescent="0.35">
@@ -14643,23 +14655,23 @@
         <v>1007</v>
       </c>
       <c r="B410" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C410" t="s">
         <v>1036</v>
       </c>
       <c r="D410" t="str">
-        <f t="shared" si="8"/>
-        <v>UF2L22_Front Left.png</v>
+        <f>E410 &amp; "_" &amp; B410 &amp; ".png"</f>
+        <v>UF2L22_Front Right.png</v>
       </c>
       <c r="E410" t="s">
         <v>1068</v>
       </c>
       <c r="F410" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="I410" s="2" t="s">
-        <v>612</v>
+        <v>459</v>
       </c>
     </row>
     <row r="411" spans="1:9" x14ac:dyDescent="0.35">
@@ -14667,26 +14679,23 @@
         <v>1007</v>
       </c>
       <c r="B411" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C411" t="s">
         <v>1036</v>
       </c>
       <c r="D411" t="str">
-        <f t="shared" si="8"/>
-        <v>UF2L23_Front Right.png</v>
+        <f>E411 &amp; "_" &amp; B411 &amp; ".png"</f>
+        <v>UF2L23_Front Left.png</v>
       </c>
       <c r="E411" t="s">
         <v>1070</v>
       </c>
       <c r="F411" t="s">
-        <v>1073</v>
-      </c>
-      <c r="G411" t="s">
-        <v>1050</v>
+        <v>1071</v>
       </c>
       <c r="I411" s="2" t="s">
-        <v>451</v>
+        <v>612</v>
       </c>
     </row>
     <row r="412" spans="1:9" x14ac:dyDescent="0.35">
@@ -14700,14 +14709,14 @@
         <v>1036</v>
       </c>
       <c r="D412" t="str">
-        <f t="shared" si="8"/>
+        <f>E412 &amp; "_" &amp; B412 &amp; ".png"</f>
         <v>UF2L24_Front Right.png</v>
       </c>
       <c r="E412" t="s">
         <v>1072</v>
       </c>
       <c r="F412" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="G412" t="s">
         <v>1050</v>
@@ -14721,26 +14730,26 @@
         <v>1007</v>
       </c>
       <c r="B413" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C413" t="s">
-        <v>1047</v>
+        <v>1036</v>
       </c>
       <c r="D413" t="str">
         <f>E413 &amp; "_" &amp; B413 &amp; ".png"</f>
-        <v>UF2L25_Front Left.png</v>
+        <v>UF2L25_Front Right.png</v>
       </c>
       <c r="E413" t="s">
         <v>1074</v>
       </c>
       <c r="F413" t="s">
-        <v>1049</v>
+        <v>1075</v>
       </c>
       <c r="G413" t="s">
         <v>1050</v>
       </c>
       <c r="I413" s="2" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="414" spans="1:9" x14ac:dyDescent="0.35">
@@ -14761,12 +14770,39 @@
         <v>1076</v>
       </c>
       <c r="F414" t="s">
-        <v>1077</v>
+        <v>1049</v>
       </c>
       <c r="G414" t="s">
         <v>1050</v>
       </c>
       <c r="I414" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="415" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A415" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B415" t="s">
+        <v>24</v>
+      </c>
+      <c r="C415" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D415" t="str">
+        <f>E415 &amp; "_" &amp; B415 &amp; ".png"</f>
+        <v>UF2L27_Front Left.png</v>
+      </c>
+      <c r="E415" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F415" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G415" t="s">
+        <v>1050</v>
+      </c>
+      <c r="I415" s="2" t="s">
         <v>459</v>
       </c>
     </row>

</xml_diff>